<commit_message>
- filled DD and DPE according to the last version of P1 in Sharepoint
</commit_message>
<xml_diff>
--- a/Franzi/DD_KARMEN_FRANZI.xlsx
+++ b/Franzi/DD_KARMEN_FRANZI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Franzi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\Franzi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC225DB-D75C-4800-9FEC-8A63D45C69F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B797BF0-C2F9-4887-90B1-6F3860042570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="106">
   <si>
     <t>index</t>
   </si>
@@ -41,13 +41,316 @@
   </si>
   <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>Kart_sum_NCI</t>
+  </si>
+  <si>
+    <t>Potatoes and potato products (incl. Fresh potatoes, heated and processed products like French fries, potato pancakes, potato chips)</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Gem02_1</t>
+  </si>
+  <si>
+    <t>Vegetables and vegetable products</t>
+  </si>
+  <si>
+    <t>Gem02_2</t>
+  </si>
+  <si>
+    <t>Mushrooms</t>
+  </si>
+  <si>
+    <t>Gem02_Hu</t>
+  </si>
+  <si>
+    <t>Legumes/Pulses (incl. lentils, chickpeas, green peas, white/broad beans, kidney/soy beans; exception: green beans; incl. canned pulses and as sauce)</t>
+  </si>
+  <si>
+    <t>Obst_sum</t>
+  </si>
+  <si>
+    <t>Fruit and fruit products (without juice) including unsweetened frozen fruit, fruit sauces and processed products like sweetened or heated fruit, canned fruit, dried fruit</t>
+  </si>
+  <si>
+    <t>Nusa_sum</t>
+  </si>
+  <si>
+    <t>Nuts and seeds (Hazelnuts, peanuts, almonds etc. or processed products like peanut butter, salted or roasted nuts)</t>
+  </si>
+  <si>
+    <t>Milc_sum</t>
+  </si>
+  <si>
+    <t>Total Dairy incl. milk and dairy products, cheese and curd cheese (incl. variants from goat, sheep)</t>
+  </si>
+  <si>
+    <t>Milc07_1</t>
+  </si>
+  <si>
+    <t>Milk and dairy products including cocoa drinks, milkshakes, yoghurt, (sour) cream, buttermilk, kefir, whey, milk powder</t>
+  </si>
+  <si>
+    <t>Fermented_milk_NCI</t>
+  </si>
+  <si>
+    <t>Fermented milk products</t>
+  </si>
+  <si>
+    <t>Milc07_2</t>
+  </si>
+  <si>
+    <t>Cheese and curd cheese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sues13_6 </t>
+  </si>
+  <si>
+    <t>Creams and desserts including pudding, semolina, tiramisu</t>
+  </si>
+  <si>
+    <t>Brot_sum</t>
+  </si>
+  <si>
+    <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls, Cereals and cereal products, Pastries</t>
+  </si>
+  <si>
+    <t>Flours_milled_prod_NCI </t>
+  </si>
+  <si>
+    <t>Flours, milled products</t>
+  </si>
+  <si>
+    <t>Pasta_rice_NCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasta, rice </t>
+  </si>
+  <si>
+    <t>Brot01_1</t>
+  </si>
+  <si>
+    <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls (incl. Crisp bread)</t>
+  </si>
+  <si>
+    <t>Bread_NCI </t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crispbread_NCI </t>
+  </si>
+  <si>
+    <t>Crispbread</t>
+  </si>
+  <si>
+    <t>Breakfast_cereals_NCI</t>
+  </si>
+  <si>
+    <t>Breakfast cereals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crackers_NCI </t>
+  </si>
+  <si>
+    <t>Crackers, breadsticks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine_bakery_NCI </t>
+  </si>
+  <si>
+    <t>Fine bakery wares</t>
+  </si>
+  <si>
+    <t>Flei_sum</t>
+  </si>
+  <si>
+    <t>Sum of meat and meat products unsmoked (including roast, goulash, schnitzel, beef olive, minced meat, meat balls, ground meat sauce) &amp; sausages and meat products smoked (including salami, liver sausage, ham, bacon, cured pork, meat loaf, bratwurst)</t>
+  </si>
+  <si>
+    <t>Flei_Wurst</t>
+  </si>
+  <si>
+    <t>Sausages and meat products smoked including salami, liver sausage, ham, bacon, cured pork, meat loaf, bratwurst</t>
+  </si>
+  <si>
+    <t>Fish_sum</t>
+  </si>
+  <si>
+    <t>Fish and fish products including salt- and freshwater fish, shrimps, mussels, snails, processed products like caviar, tinned fish</t>
+  </si>
+  <si>
+    <t>Eier_sum_NCI</t>
+  </si>
+  <si>
+    <t>Eggs and egg products including scrambled, fried and boiled eggs, omelets, soufflé</t>
+  </si>
+  <si>
+    <t>Fett_sum</t>
+  </si>
+  <si>
+    <t>fats &amp; oils (excl: in salad dressings) - incl. Animal-based fats, plant-based fats and not specified fats/öls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veg_fatsoils_NCI </t>
+  </si>
+  <si>
+    <t>Vegetable fats and oils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butter_NCI </t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marg_Streichf_NCI </t>
+  </si>
+  <si>
+    <t>Margarine and similar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal_fatsoils_NCI </t>
+  </si>
+  <si>
+    <t>Animal fats excluding butter, fish oil</t>
+  </si>
+  <si>
+    <t>Sues_sum</t>
+  </si>
+  <si>
+    <t>Sweets (sum)</t>
+  </si>
+  <si>
+    <t>Sues13_1</t>
+  </si>
+  <si>
+    <t>Sweets including sweets with chocolate, confectionaries, candies, fruit gums, cereal bars</t>
+  </si>
+  <si>
+    <t>Sues13_2</t>
+  </si>
+  <si>
+    <t>Ice cream</t>
+  </si>
+  <si>
+    <t>Cakes_NCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cakes </t>
+  </si>
+  <si>
+    <t>Getr15_1</t>
+  </si>
+  <si>
+    <t>non-alcoholic beverages (sum)</t>
+  </si>
+  <si>
+    <t>Getr15_14</t>
+  </si>
+  <si>
+    <t>Fruit juices/nectars (incl. Spritzer) - excl. vegetable juices</t>
+  </si>
+  <si>
+    <t>Getr15_16</t>
+  </si>
+  <si>
+    <t>Soft drinks e.g. lemonades, bitter lemon (incl. low-calorie drinks)</t>
+  </si>
+  <si>
+    <t>Getr15_11</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Getr15_12</t>
+  </si>
+  <si>
+    <t>Coffee + Tea (black/green)</t>
+  </si>
+  <si>
+    <t>Getr15_13</t>
+  </si>
+  <si>
+    <t>Herbal/fruit tea</t>
+  </si>
+  <si>
+    <t>Getr15_2</t>
+  </si>
+  <si>
+    <t>Alcoholic beverages (sum)</t>
+  </si>
+  <si>
+    <t>Getr15_22</t>
+  </si>
+  <si>
+    <t>Wine and sparkling wine</t>
+  </si>
+  <si>
+    <t>Getr15_21</t>
+  </si>
+  <si>
+    <t>Beer including mixed beer drinks</t>
+  </si>
+  <si>
+    <t>Getr15_23</t>
+  </si>
+  <si>
+    <t>spirits incl. schnapps, liqueurs</t>
+  </si>
+  <si>
+    <t>Getr15_24</t>
+  </si>
+  <si>
+    <t>Other alcoholic beverages e.g. alcopops, cocktails</t>
+  </si>
+  <si>
+    <t>Sose_sum</t>
+  </si>
+  <si>
+    <t>Sauces including warm and cold sauces (e.g. ketchup, salad dressing), mustard, vinegar etc.; exceptions: fruit-, vegetable-, ground meat sauce</t>
+  </si>
+  <si>
+    <t>Supp_sum</t>
+  </si>
+  <si>
+    <t>Soups without stews</t>
+  </si>
+  <si>
+    <t>Sonst_sum</t>
+  </si>
+  <si>
+    <t>Milk substitutes (e.g. soy products (milk, yoghurt, cheese), coconut-, rice-, oat-, almond milk, cereal milk with soy), meat substitutes (e.g. tofu, tempeh, soy protein, vegetarian sausages), cereal substitutes (e.g. soy flour/flakes, lupines), sweeteners, sugar substitutes, beverage powders/ -granules (e.g. cocoa powder, lemonade powder), herbs, spices, vegetarian spreads, protein powder, yeast, miso</t>
+  </si>
+  <si>
+    <t>Veg_products_NCI</t>
+  </si>
+  <si>
+    <t>Vegetarian products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soyproducts_NCI </t>
+  </si>
+  <si>
+    <t>Soyproducts</t>
+  </si>
+  <si>
+    <t>Suessstoffe</t>
+  </si>
+  <si>
+    <t>table sweeteners (low/no caloric sweeteners) (excl. Stevia)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +366,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,9 +443,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -119,7 +477,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -417,11 +775,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
@@ -444,304 +802,704 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51"/>
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52"/>
@@ -1011,11 +1769,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
@@ -1040,15 +1798,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -1058,6 +1807,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1302,14 +2060,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1322,6 +2072,14 @@
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DD_KARMEN_FRANZI + DPE_KARMEN_FRANZI: removed whitespace and index
</commit_message>
<xml_diff>
--- a/Franzi/DD_KARMEN_FRANZI.xlsx
+++ b/Franzi/DD_KARMEN_FRANZI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\Franzi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Franzi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B797BF0-C2F9-4887-90B1-6F3860042570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558CB11B-9A6F-4A1D-98EA-A4B1362813AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls, Cereals and cereal products, Pastries</t>
   </si>
   <si>
-    <t>Flours_milled_prod_NCI </t>
-  </si>
-  <si>
     <t>Flours, milled products</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Sum of Wholemeal bread/rolls, White, brown or multigrain bread/rolls (incl. Crisp bread)</t>
   </si>
   <si>
-    <t>Bread_NCI </t>
-  </si>
-  <si>
     <t>Bread</t>
   </si>
   <si>
@@ -344,6 +338,12 @@
   </si>
   <si>
     <t>table sweeteners (low/no caloric sweeteners) (excl. Stevia)</t>
+  </si>
+  <si>
+    <t>Flours_milled_prod_NCI</t>
+  </si>
+  <si>
+    <t>Bread_NCI</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -477,7 +477,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -775,11 +775,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="3"/>
     <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
@@ -802,9 +802,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
+      <c r="A2"/>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
@@ -816,9 +814,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
+      <c r="A3"/>
       <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
@@ -830,9 +826,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
+      <c r="A4"/>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
@@ -844,9 +838,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
+      <c r="A5"/>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -858,9 +850,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
+      <c r="A6"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -872,9 +862,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
+      <c r="A7"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
@@ -886,9 +874,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
+      <c r="A8"/>
       <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
@@ -900,9 +886,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
+      <c r="A9"/>
       <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
@@ -914,9 +898,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
+      <c r="A10"/>
       <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
@@ -928,9 +910,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
+      <c r="A11"/>
       <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
@@ -942,9 +922,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
+      <c r="A12"/>
       <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
@@ -956,9 +934,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
+      <c r="A13"/>
       <c r="B13" s="8" t="s">
         <v>28</v>
       </c>
@@ -970,791 +946,665 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
+      <c r="A14"/>
       <c r="B14" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="D18" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
+      <c r="D20" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="D21" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="D22" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="D23" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="D24" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="D25" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="8" t="s">
+      <c r="D26" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="D28" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="D29" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="D30" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="8" t="s">
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="11" t="s">
+      <c r="D32" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="8" t="s">
+      <c r="D33" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="D34" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="8" t="s">
+      <c r="D35" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" s="8" t="s">
+      <c r="D36" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" s="8" t="s">
+      <c r="D37" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="8" t="s">
+      <c r="D38" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="11" t="s">
+      <c r="D39" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="8" t="s">
+      <c r="D40" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" s="8" t="s">
+      <c r="D41" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" s="8" t="s">
+      <c r="D42" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" s="8" t="s">
+      <c r="D43" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" s="8" t="s">
+      <c r="D44" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="8" t="s">
+      <c r="D45" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" s="8" t="s">
+      <c r="D46" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="D47" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="D48" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" s="7" t="s">
+      <c r="D49" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" s="7" t="s">
+      <c r="D50" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="D51" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52"/>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53"/>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54"/>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55"/>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56"/>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57"/>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58"/>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59"/>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60"/>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61"/>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62"/>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63"/>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64"/>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65"/>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66"/>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67"/>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68"/>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69"/>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70"/>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71"/>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72"/>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73"/>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74"/>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75"/>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76"/>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77"/>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78"/>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79"/>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80"/>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81"/>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82"/>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83"/>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84"/>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85"/>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86"/>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87"/>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88"/>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89"/>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90"/>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91"/>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92"/>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93"/>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94"/>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
@@ -1773,7 +1623,7 @@
       <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
@@ -1810,15 +1660,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -2059,6 +1900,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
@@ -2077,14 +1927,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607F74A7-32EE-406C-A688-0D84C4E12BE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2101,4 +1943,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>